<commit_message>
Filtrado de datos, txt de entrada
</commit_message>
<xml_diff>
--- a/Datos/Tier_List_Cartas.xlsx
+++ b/Datos/Tier_List_Cartas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CF9FBC-2962-4942-A1E1-4BD937B976D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CC7C31-706F-4938-B38D-7E8DBBFD5F45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +443,7 @@
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -498,6 +499,9 @@
       </c>
       <c r="H2">
         <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>